<commit_message>
Se restaura Caso de uso 20
</commit_message>
<xml_diff>
--- a/se/Trabajo Profesional/Disciplinas/3.Analisis/Casos de Uso/CU20 - Ingresando al sistema/TC20 - Ingresando al sistema.xlsx
+++ b/se/Trabajo Profesional/Disciplinas/3.Analisis/Casos de Uso/CU20 - Ingresando al sistema/TC20 - Ingresando al sistema.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="18990" windowHeight="8280"/>
@@ -220,8 +220,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,103 +507,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <condense val="0"/>
@@ -761,7 +665,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -796,7 +699,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -972,17 +874,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P1048569"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
@@ -1001,7 +903,7 @@
     <col min="22" max="22" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="15" customFormat="1">
       <c r="A1" s="28"/>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -1023,7 +925,7 @@
       <c r="O1" s="32"/>
       <c r="P1" s="5"/>
     </row>
-    <row r="2" spans="1:16" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="15" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1065,7 +967,7 @@
       </c>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="45">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -1095,7 +997,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="45">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
@@ -1125,7 +1027,7 @@
       <c r="O4" s="11"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="45">
       <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>20</v>
@@ -1155,7 +1057,7 @@
       <c r="O5" s="11"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="30">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>20</v>
@@ -1185,7 +1087,7 @@
       <c r="O6" s="11"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="45">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>17</v>
@@ -1215,7 +1117,7 @@
       <c r="O7" s="11"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" s="12"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1233,7 +1135,7 @@
       <c r="O8" s="11"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" s="12"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1251,7 +1153,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" s="12"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1269,7 +1171,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" s="12"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1287,7 +1189,7 @@
       <c r="O11" s="11"/>
       <c r="P11" s="8"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="12"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1305,7 +1207,7 @@
       <c r="O12" s="11"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="12"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1323,7 +1225,7 @@
       <c r="O13" s="11"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="12"/>
       <c r="B14" s="2"/>
       <c r="C14" s="9"/>
@@ -1341,7 +1243,7 @@
       <c r="O14" s="11"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="12"/>
       <c r="B15" s="2"/>
       <c r="C15" s="9"/>
@@ -1359,7 +1261,7 @@
       <c r="O15" s="11"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="12"/>
       <c r="B16" s="2"/>
       <c r="C16" s="9"/>
@@ -1377,7 +1279,7 @@
       <c r="O16" s="11"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="12"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1395,7 +1297,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="12"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1413,7 +1315,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="12"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1429,7 +1331,7 @@
       <c r="N19" s="17"/>
       <c r="O19" s="10"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="22"/>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -1440,7 +1342,7 @@
       <c r="H20" s="22"/>
       <c r="I20" s="23"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="22"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -1451,7 +1353,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="23"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="22"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -1462,7 +1364,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="23"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" s="22"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -1473,7 +1375,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="23"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" s="22"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -1484,22 +1386,22 @@
       <c r="H24" s="22"/>
       <c r="I24" s="23"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" s="25"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" s="25"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" s="25"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16">
       <c r="A28" s="24"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16">
       <c r="A29" s="24"/>
     </row>
-    <row r="1048569" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="1048569" spans="6:6">
       <c r="F1048569" s="2"/>
     </row>
   </sheetData>
@@ -1515,18 +1417,18 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="G2:G6 G8:G24">
-    <cfRule type="cellIs" dxfId="11" priority="195" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="195" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="196" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="196" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N19">
-    <cfRule type="cellIs" dxfId="9" priority="193" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="193" stopIfTrue="1" operator="equal">
       <formula>"TEST OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="194" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="194" stopIfTrue="1" operator="equal">
       <formula>"TEST FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1639,10 +1541,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"True"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"False"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>